<commit_message>
- Added static type hinting.\n-Fixed little problems with merkle root
</commit_message>
<xml_diff>
--- a/T-Project Product features.xlsx
+++ b/T-Project Product features.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>ID</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>consensus</t>
+  </si>
+  <si>
+    <t>create coin addresses like bitcoin</t>
   </si>
 </sst>
 </file>
@@ -196,8 +199,8 @@
       <sheetName val="Parameters"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
       <sheetData sheetId="2">
         <row r="2">
           <cell r="A2" t="str">
@@ -609,7 +612,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,12 +704,14 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>

</xml_diff>